<commit_message>
Modify tests, fix bugs. Rename modules.
</commit_message>
<xml_diff>
--- a/data/railway_od_pairs_current.xlsx
+++ b/data/railway_od_pairs_current.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$2458</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
   <si>
     <t>30-45</t>
   </si>
@@ -143,6 +143,288 @@
   </si>
   <si>
     <t>24-21</t>
+  </si>
+  <si>
+    <t>92-94</t>
+  </si>
+  <si>
+    <t>22-23</t>
+  </si>
+  <si>
+    <t>33-34</t>
+  </si>
+  <si>
+    <t>1-1003</t>
+  </si>
+  <si>
+    <t>23-33</t>
+  </si>
+  <si>
+    <t>7-92</t>
+  </si>
+  <si>
+    <t>8-35</t>
+  </si>
+  <si>
+    <t>73-1003</t>
+  </si>
+  <si>
+    <t>7-95</t>
+  </si>
+  <si>
+    <t>60-1059</t>
+  </si>
+  <si>
+    <t>44-97</t>
+  </si>
+  <si>
+    <t>63-83</t>
+  </si>
+  <si>
+    <t>56-58</t>
+  </si>
+  <si>
+    <t>5-91</t>
+  </si>
+  <si>
+    <t>33-92</t>
+  </si>
+  <si>
+    <t>36-37</t>
+  </si>
+  <si>
+    <t>38-59</t>
+  </si>
+  <si>
+    <t>68-69</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>1-91</t>
+  </si>
+  <si>
+    <t>3-27</t>
+  </si>
+  <si>
+    <t>8-47</t>
+  </si>
+  <si>
+    <t>19-22</t>
+  </si>
+  <si>
+    <t>8-97</t>
+  </si>
+  <si>
+    <t>23-42</t>
+  </si>
+  <si>
+    <t>3-51</t>
+  </si>
+  <si>
+    <t>4-95</t>
+  </si>
+  <si>
+    <t>56-60</t>
+  </si>
+  <si>
+    <t>25-46</t>
+  </si>
+  <si>
+    <t>34-42</t>
+  </si>
+  <si>
+    <t>63-64</t>
+  </si>
+  <si>
+    <t>69-1003</t>
+  </si>
+  <si>
+    <t>23-38</t>
+  </si>
+  <si>
+    <t>8-99</t>
+  </si>
+  <si>
+    <t>17-71</t>
+  </si>
+  <si>
+    <t>46-83</t>
+  </si>
+  <si>
+    <t>8-38</t>
+  </si>
+  <si>
+    <t>67-68</t>
+  </si>
+  <si>
+    <t>41-59</t>
+  </si>
+  <si>
+    <t>14-57</t>
+  </si>
+  <si>
+    <t>49-56</t>
+  </si>
+  <si>
+    <t>43-97</t>
+  </si>
+  <si>
+    <t>3-26</t>
+  </si>
+  <si>
+    <t>1-1021</t>
+  </si>
+  <si>
+    <t>21-1021</t>
+  </si>
+  <si>
+    <t>1022-1052</t>
+  </si>
+  <si>
+    <t>91-1020</t>
+  </si>
+  <si>
+    <t>55-91</t>
+  </si>
+  <si>
+    <t>4-14</t>
+  </si>
+  <si>
+    <t>8-48</t>
+  </si>
+  <si>
+    <t>66-79</t>
+  </si>
+  <si>
+    <t>77-78</t>
+  </si>
+  <si>
+    <t>17-1011</t>
+  </si>
+  <si>
+    <t>12-73</t>
+  </si>
+  <si>
+    <t>13-71</t>
+  </si>
+  <si>
+    <t>22-52</t>
+  </si>
+  <si>
+    <t>40-92</t>
+  </si>
+  <si>
+    <t>19-23</t>
+  </si>
+  <si>
+    <t>33-97</t>
+  </si>
+  <si>
+    <t>34-43</t>
+  </si>
+  <si>
+    <t>60-95</t>
+  </si>
+  <si>
+    <t>56-65</t>
+  </si>
+  <si>
+    <t>24-49</t>
+  </si>
+  <si>
+    <t>48-97</t>
+  </si>
+  <si>
+    <t>2-1059</t>
+  </si>
+  <si>
+    <t>56-92</t>
+  </si>
+  <si>
+    <t>77-81</t>
+  </si>
+  <si>
+    <t>57-64</t>
+  </si>
+  <si>
+    <t>37-83</t>
+  </si>
+  <si>
+    <t>66-1001</t>
+  </si>
+  <si>
+    <t>25-49</t>
+  </si>
+  <si>
+    <t>11-73</t>
+  </si>
+  <si>
+    <t>56-1060</t>
+  </si>
+  <si>
+    <t>77-80</t>
+  </si>
+  <si>
+    <t>60-1060</t>
+  </si>
+  <si>
+    <t>13-70</t>
+  </si>
+  <si>
+    <t>22-1037</t>
+  </si>
+  <si>
+    <t>71-1012</t>
+  </si>
+  <si>
+    <t>69-1012</t>
+  </si>
+  <si>
+    <t>23-24</t>
+  </si>
+  <si>
+    <t>49-1022</t>
+  </si>
+  <si>
+    <t>49-1023</t>
+  </si>
+  <si>
+    <t>19-43</t>
+  </si>
+  <si>
+    <t>55-64</t>
+  </si>
+  <si>
+    <t>55-56</t>
+  </si>
+  <si>
+    <t>68-79</t>
+  </si>
+  <si>
+    <t>56-89</t>
+  </si>
+  <si>
+    <t>51-1023</t>
+  </si>
+  <si>
+    <t>10-92</t>
+  </si>
+  <si>
+    <t>41-44</t>
+  </si>
+  <si>
+    <t>9-92</t>
+  </si>
+  <si>
+    <t>5-23</t>
+  </si>
+  <si>
+    <t>66-81</t>
+  </si>
+  <si>
+    <t>3-43</t>
   </si>
 </sst>
 </file>
@@ -487,7 +769,7 @@
   <dimension ref="A1:D5304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,327 +1598,797 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
+      <c r="A101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1760200</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
+      <c r="A102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1056188</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
+      <c r="A103" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" s="3">
+        <v>747500</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
+      <c r="A104" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B104" s="3">
+        <v>547800</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3"/>
+      <c r="A105" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="3">
+        <v>544966.78</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="3"/>
+      <c r="A106" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106" s="3">
+        <v>525676.78</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="3"/>
+      <c r="A107" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" s="3">
+        <v>471153.64</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
+      <c r="A108" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B108" s="3">
+        <v>443300</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
+      <c r="A109" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="3">
+        <v>420390.21</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="3"/>
+      <c r="A110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110" s="3">
+        <v>417600</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="3"/>
+      <c r="A111" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" s="3">
+        <v>379269.4</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="3"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="3"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="3"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="3"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="3"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="3"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="3"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="3"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="3"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="3"/>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="3"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="3"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="3"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="3"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="3"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="3"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="3"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="3"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="3"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="3"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="3"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="3"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="3"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="3"/>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="3"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="3"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="3"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="3"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="3"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="3"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3"/>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="3"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="3"/>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="3"/>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="3"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="3"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="3"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="3"/>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="3"/>
-    </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="3"/>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="3">
+        <v>369953.46</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="3">
+        <v>277638.37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" s="3">
+        <v>270832.71000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B115" s="3">
+        <v>266533.21999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B116" s="3">
+        <v>263200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B117" s="3">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B118" s="3">
+        <v>227700</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B119" s="3">
+        <v>225366.86</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B120" s="3">
+        <v>216467.29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B121" s="3">
+        <v>198197.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B122" s="3">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" s="3">
+        <v>185524.46</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B124" s="3">
+        <v>181979.39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B125" s="3">
+        <v>176700.57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B126" s="3">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B127" s="3">
+        <v>163224.34</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B128" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" s="3">
+        <v>147184.04999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B130" s="3">
+        <v>132715.46</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="3">
+        <v>125359.69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B132" s="3">
+        <v>104500</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B133" s="3">
+        <v>100465.79</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B134" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B135" s="3">
+        <v>96800</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B136" s="3">
+        <v>90523.971999999994</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B137" s="3">
+        <v>87500</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B138" s="3">
+        <v>81794.334000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B139" s="3">
+        <v>77500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B140" s="3">
+        <v>77011.194000000003</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B141" s="3">
+        <v>77010</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B142" s="3">
+        <v>75118.187000000005</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B143" s="3">
+        <v>75016</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B144" s="3">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" s="3">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B146" s="3">
+        <v>66520.254000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B147" s="3">
+        <v>63500</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B148" s="3">
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B149" s="3">
+        <v>62142.519</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150" s="3">
+        <v>60366.972000000002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B151" s="3">
+        <v>58044.334000000003</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B152" s="3">
+        <v>57250</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B153" s="3">
+        <v>57200</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B154" s="3">
+        <v>56100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B155" s="3">
+        <v>56100</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B156" s="3">
+        <v>52187.514999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B157" s="3">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B158" s="3">
+        <v>49975.902000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B159" s="3">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B160" s="3">
+        <v>47284.544000000002</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B161" s="3">
+        <v>46485.449000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B162" s="3">
+        <v>45068.192999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B163" s="3">
+        <v>43710.050999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B164" s="3">
+        <v>42133.027999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B165" s="3">
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B166" s="3">
+        <v>39490</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B167" s="3">
+        <v>36500</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B168" s="3">
+        <v>36261.805999999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B169" s="3">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B170" s="3">
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B171" s="3">
+        <v>34648.453999999998</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B172" s="3">
+        <v>34100</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B173" s="3">
+        <v>33500</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B174" s="3">
+        <v>31250</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B175" s="3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" s="3">
+        <v>25300</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B177" s="3">
+        <v>22100</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B178" s="3">
+        <v>20900</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B179" s="3">
+        <v>18700</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B180" s="3">
+        <v>16732.468000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B181" s="3">
+        <v>14679.745999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B182" s="3">
+        <v>13049.767</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B183" s="3">
+        <v>11914</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B184" s="3">
+        <v>11750</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B185" s="3">
+        <v>11750</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B186" s="3">
+        <v>10955.665999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B187" s="3">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B188" s="3">
+        <v>8396.1929999999993</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B189" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B190" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B191" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B192" s="3">
+        <v>2167.2865000000002</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B193" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B194" s="3">
+        <v>919.64323999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>